<commit_message>
eliminar duplicados filtrados por email
se añade subset para eliminar duplicados filtrados por email
</commit_message>
<xml_diff>
--- a/nombres_email.xlsx
+++ b/nombres_email.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAC6A114-CDC0-4516-AD8F-32D7C085ADC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760AC774-90F1-47FB-B20B-83930C02DE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6795" yWindow="2055" windowWidth="18840" windowHeight="10620" xr2:uid="{1C4F3AAD-3B23-4D6E-8B35-84F3403F6B74}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>ddd@ddd.com</t>
+  </si>
+  <si>
+    <t>aaa1</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +453,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>

</xml_diff>